<commit_message>
update gpio_config_builder.py and gpio_config_io.c to not generate n_bits value
</commit_message>
<xml_diff>
--- a/hardware/caravel_Nucleo/caravel_Nucleo.xlsx
+++ b/hardware/caravel_Nucleo/caravel_Nucleo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Efabless\caravel_board\hardware\caravel_Nucleo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffdi/Projects/caravel_board/hardware/caravel_nucleo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FA8050-D696-4FFC-92C7-C547F991E859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4338B9-D4E9-FA43-ABAB-2DE295A41312}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="2960" windowWidth="19200" windowHeight="11170" xr2:uid="{DBB590BE-7B6D-5543-BF5E-2321E179B520}"/>
+    <workbookView xWindow="17700" yWindow="4760" windowWidth="28320" windowHeight="19480" xr2:uid="{DBB590BE-7B6D-5543-BF5E-2321E179B520}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="3" r:id="rId1"/>
@@ -222,9 +222,6 @@
     <t>R25, R26</t>
   </si>
   <si>
-    <t>R29-R32</t>
-  </si>
-  <si>
     <t>TP1</t>
   </si>
   <si>
@@ -274,6 +271,9 @@
   </si>
   <si>
     <t>TAR5S18UTE85LF</t>
+  </si>
+  <si>
+    <t>R29-R33</t>
   </si>
 </sst>
 </file>
@@ -704,15 +704,15 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="27.33203125" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" style="7" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
-    <col min="6" max="6" width="13.58203125" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -756,7 +756,7 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>13</v>
@@ -774,7 +774,7 @@
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>13</v>
@@ -783,7 +783,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" s="6">
         <v>2</v>
@@ -802,11 +802,11 @@
         <v>0</v>
       </c>
       <c r="B6" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>13</v>
@@ -819,7 +819,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="8" t="s">
@@ -855,7 +855,7 @@
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>12</v>
@@ -863,14 +863,14 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" s="6">
         <v>1</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>13</v>
@@ -878,14 +878,14 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" s="6">
         <v>1</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>13</v>
@@ -1021,7 +1021,7 @@
         <v>55</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E19" t="s">
         <v>13</v>
@@ -1038,7 +1038,7 @@
         <v>57</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E20" t="s">
         <v>13</v>
@@ -1055,7 +1055,7 @@
         <v>61</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E21" t="s">
         <v>13</v>
@@ -1072,7 +1072,7 @@
         <v>59</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E22" t="s">
         <v>13</v>
@@ -1089,7 +1089,7 @@
         <v>499</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E23" t="s">
         <v>13</v>
@@ -1106,7 +1106,7 @@
         <v>360</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E24" t="s">
         <v>13</v>
@@ -1148,16 +1148,16 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="B27" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C27" s="4">
         <v>0</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E27" t="s">
         <v>13</v>
@@ -1214,7 +1214,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B31" s="7">
         <v>1</v>

</xml_diff>

<commit_message>
update gpio_config and Matt's example
</commit_message>
<xml_diff>
--- a/hardware/caravel_Nucleo/caravel_Nucleo.xlsx
+++ b/hardware/caravel_Nucleo/caravel_Nucleo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffdi/Projects/caravel_board/hardware/caravel_nucleo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffdi/Projects/caravel_board/hardware/caravel_Nucleo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4338B9-D4E9-FA43-ABAB-2DE295A41312}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FD563D-C90E-EE40-A3FE-42F1B621A934}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17700" yWindow="4760" windowWidth="28320" windowHeight="19480" xr2:uid="{DBB590BE-7B6D-5543-BF5E-2321E179B520}"/>
+    <workbookView xWindow="17000" yWindow="3320" windowWidth="28320" windowHeight="19480" xr2:uid="{DBB590BE-7B6D-5543-BF5E-2321E179B520}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="94">
   <si>
     <t>U6</t>
   </si>
@@ -274,6 +274,45 @@
   </si>
   <si>
     <t>R29-R33</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>J8, J9</t>
+  </si>
+  <si>
+    <t>Alps Alpine </t>
+  </si>
+  <si>
+    <t>SKQGADE010</t>
+  </si>
+  <si>
+    <t>SSQ-126-23-G-D</t>
+  </si>
+  <si>
+    <t>70-pin 2-row socket</t>
+  </si>
+  <si>
+    <t>UNMARKED - connectors on board edge</t>
+  </si>
+  <si>
+    <t>3-pin straight header</t>
+  </si>
+  <si>
+    <t>77311-118-03LF</t>
+  </si>
+  <si>
+    <t>mouser</t>
+  </si>
+  <si>
+    <t>NOTE - install on backside of PCB</t>
+  </si>
+  <si>
+    <t>FlexyPins</t>
+  </si>
+  <si>
+    <t>see link</t>
   </si>
 </sst>
 </file>
@@ -360,7 +399,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -385,6 +424,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -701,16 +741,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{718CFFD5-71E2-E44C-BCD6-97EE3DEEFA9F}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="27.33203125" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
   </cols>
@@ -976,7 +1017,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -993,7 +1034,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -1010,7 +1051,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1027,7 +1068,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -1044,7 +1085,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>62</v>
       </c>
@@ -1061,7 +1102,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -1078,7 +1119,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -1095,7 +1136,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -1112,7 +1153,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1129,7 +1170,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -1146,7 +1187,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>80</v>
       </c>
@@ -1163,7 +1204,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1">
+    <row r="28" spans="1:6" ht="15" customHeight="1">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -1178,7 +1219,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -1195,7 +1236,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -1212,7 +1253,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -1225,6 +1266,77 @@
       </c>
       <c r="E31" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="7">
+        <v>1</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" t="s">
+        <v>90</v>
+      </c>
+      <c r="F32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" s="7">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" s="7">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E34" t="s">
+        <v>90</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="7">
+        <v>50</v>
+      </c>
+      <c r="C35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E35" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1257,8 +1369,12 @@
     <hyperlink ref="D24" r:id="rId26" xr:uid="{B3F54C6A-C353-47E5-8E7A-71305346B02D}"/>
     <hyperlink ref="D28" r:id="rId27" xr:uid="{ECA5F3D5-98AA-46FB-B542-A4223E5D1F67}"/>
     <hyperlink ref="D27" r:id="rId28" xr:uid="{C3FE6C8E-A4F6-4D82-9AB1-A35F502480E9}"/>
+    <hyperlink ref="D32" r:id="rId29" xr:uid="{5DE7BAB7-DE90-7B41-B726-127624F7369E}"/>
+    <hyperlink ref="D34" r:id="rId30" xr:uid="{7CE7225A-BB7C-7F47-BD6E-16B23076998B}"/>
+    <hyperlink ref="D33" r:id="rId31" xr:uid="{4E2E7D93-AC74-DA45-AAB3-4D595D6DB6A9}"/>
+    <hyperlink ref="D35" r:id="rId32" xr:uid="{E293F2F3-6C58-5E4C-BCD9-AC6B5545F9B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId29"/>
+  <pageSetup orientation="portrait" r:id="rId33"/>
 </worksheet>
 </file>
</xml_diff>